<commit_message>
some more scripts got added
</commit_message>
<xml_diff>
--- a/OnboardingAppFramework/testdata/onboardingTestScriptData.xlsx
+++ b/OnboardingAppFramework/testdata/onboardingTestScriptData.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7770"/>
+    <workbookView windowWidth="14550" windowHeight="6075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <oleSize ref="A2:G11"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1554,7 +1555,7 @@
   <sheetPr/>
   <dimension ref="A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1579,7 +1580,7 @@
   <sheetPr/>
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>

</xml_diff>